<commit_message>
adding COVID 19 Project to Github
</commit_message>
<xml_diff>
--- a/Info on Data Origin.xlsx
+++ b/Info on Data Origin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bench\Downloads\STAT 222\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasmin/Desktop/!STAT MA 2020/!222/COVID-19-Economics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FCF84D-8D9E-47C1-8FE3-C543EFD58917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1A55D8-52E0-134B-8702-58DD1E8A16F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{937BE5BC-62DF-4A63-9F82-E4C1CBA98BA1}"/>
+    <workbookView xWindow="15900" yWindow="3320" windowWidth="29040" windowHeight="16000" xr2:uid="{937BE5BC-62DF-4A63-9F82-E4C1CBA98BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Dataset</t>
   </si>
@@ -60,9 +60,6 @@
     <t>https://www.bls.gov/web/laus.supp.toc.htm</t>
   </si>
   <si>
-    <t>UnemploySA.csv</t>
-  </si>
-  <si>
     <t>uscases.csv</t>
   </si>
   <si>
@@ -96,14 +93,104 @@
     <t>US Unemployment Rate on a Micro level (Sex, Race)</t>
   </si>
   <si>
-    <t>Overall and State Unemployment Rate (Season-Adj)</t>
+    <t>https://www.bls.gov/data/#prices</t>
+  </si>
+  <si>
+    <t>US CPI</t>
+  </si>
+  <si>
+    <t>cpi_all_adj.csv, cpi_all_notadj.csv, cpi_lessfood_adj.csv, cpi_lessfood_notadj.csv</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/DPRIME</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/FEDFUNDS</t>
+  </si>
+  <si>
+    <t>US Prime Rate</t>
+  </si>
+  <si>
+    <t>US Federal Funds Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Fed </t>
+  </si>
+  <si>
+    <t>DPRIME.csv</t>
+  </si>
+  <si>
+    <t>FEDFUNDS.csv</t>
+  </si>
+  <si>
+    <t>US Court</t>
+  </si>
+  <si>
+    <t>bankruptcy_california.xlsx</t>
+  </si>
+  <si>
+    <t>California Bankruptcy Filings (manually created data set using Table F-2)</t>
+  </si>
+  <si>
+    <t>https://www.uscourts.gov/statistics/table/f-2-three-months/bankruptcy-filings/2020/12/31</t>
+  </si>
+  <si>
+    <t>stringency_us</t>
+  </si>
+  <si>
+    <t>Oxford U.</t>
+  </si>
+  <si>
+    <t>https://github.com/OxCGRT/USA-covid-policy</t>
+  </si>
+  <si>
+    <t>Stringency data of U.S.</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>reliability - subject to discussion</t>
+  </si>
+  <si>
+    <t>unemployment_sector_NSA</t>
+  </si>
+  <si>
+    <t>Fed Reserve STL</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/categories/32447?cid=32447&amp;et=&amp;ob=pv&amp;od=desc&amp;pageID=1&amp;t=monthly</t>
+  </si>
+  <si>
+    <t>Unemployment Rate by Sector (Non Season-Adj)</t>
+  </si>
+  <si>
+    <t>UnemployNSA.csv</t>
+  </si>
+  <si>
+    <t>State Unemployment Rate (Non-Season-Adj)</t>
+  </si>
+  <si>
+    <t>https://apps.bea.gov/iTable/iTable.cfm?reqid=70&amp;step=1&amp;acrdn=4</t>
+  </si>
+  <si>
+    <t>bea</t>
+  </si>
+  <si>
+    <t>sector employment numbers by state</t>
+  </si>
+  <si>
+    <t>state_sector</t>
+  </si>
+  <si>
+    <t>just used for presentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +202,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,6 +244,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,35 +561,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC7FDF7-BFAD-46F5-B881-5A5BFB5DED36}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -503,12 +604,12 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -517,67 +618,167 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{91386543-934F-4E50-BAAD-73027CF3549B}"/>
+    <hyperlink ref="C20" r:id="rId2" location="prices" xr:uid="{92CBE02A-D8F0-4D49-B803-641999C18EE5}"/>
+    <hyperlink ref="C21" r:id="rId3" xr:uid="{43E53EB2-1EAF-A840-A98A-759B7A905DFD}"/>
+    <hyperlink ref="C22" r:id="rId4" xr:uid="{F69D4B89-A906-9844-A716-08C2BAECD6AB}"/>
+    <hyperlink ref="C23" r:id="rId5" xr:uid="{17A27A6F-338B-FF43-8288-6EB60C35EF1D}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{35EBF059-929B-734E-9D6E-8DD1D8391201}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{228F8651-FA4B-4B40-AB49-14352A6D5B9A}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{28A320C2-F57C-7B4E-AAF2-B59574EFFABD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>